<commit_message>
Corrected error in MSW O&M and constructions costs
</commit_message>
<xml_diff>
--- a/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
+++ b/InputData/elec/CCaMC/Capacity Construction and Maint Costs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\World Resources Institute\TRAC City - HK 2050 is now\EPS HK 2.0\eps-2.0.0-us-wipF\InputData\elec\CCaMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-hongkong\InputData\elec\CCaMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{49BBDC4E-F4A1-4D4E-9667-F7F2C2294AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FF8CC6B-EB11-4C87-B3A4-8C7B1D6D7500}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -26,12 +25,14 @@
     <sheet name="CCaMC-VOaMCpUC" sheetId="8" r:id="rId11"/>
     <sheet name="CCaMC-BCCpUC" sheetId="6" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="418">
   <si>
     <t>CCaMC BAU Construction Cost per Unit Capacity</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -1530,9 +1531,6 @@
     <t>MW</t>
   </si>
   <si>
-    <t xml:space="preserve">cost </t>
-  </si>
-  <si>
     <t>Fixed O&amp;M ($/MW)</t>
   </si>
   <si>
@@ -1594,21 +1592,190 @@
   </si>
   <si>
     <t>Offshore Wind ($/MW)</t>
+  </si>
+  <si>
+    <t>billion USD/year</t>
+  </si>
+  <si>
+    <t>municipal solid waste ($/MW)</t>
+  </si>
+  <si>
+    <t>https://www.legco.gov.hk/yr13-14/english/fc/pwsc/papers/p14-07e.pdf</t>
+  </si>
+  <si>
+    <t>ITEM FOR PUBLIC WORKS SUBCOMMITTEE
+OF FINANCE COMMITTEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We estimate the capital cost of the proposed works to be $18,245.7 million
+in MOD prices (please see paragraph 13 below), broken down as follows – </t>
+  </si>
+  <si>
+    <t>$ million</t>
+  </si>
+  <si>
+    <t>(a) Reclamation and civil works</t>
+  </si>
+  <si>
+    <t>(i) Seawall, reclamation and berth</t>
+  </si>
+  <si>
+    <t>(ii) Breakwaters</t>
+  </si>
+  <si>
+    <t>(iii) Civil and foundation works</t>
+  </si>
+  <si>
+    <t>(b) Building and architectural works</t>
+  </si>
+  <si>
+    <t>(i) Incineration plant building</t>
+  </si>
+  <si>
+    <t>(ii) Mechanical plant building</t>
+  </si>
+  <si>
+    <t>(iii) Associated buildings</t>
+  </si>
+  <si>
+    <t>(iv) Landscaping</t>
+  </si>
+  <si>
+    <t>(c) Mechanical and electrical works for incineration</t>
+  </si>
+  <si>
+    <t>(i) Waste receiving facilities</t>
+  </si>
+  <si>
+    <t>(ii) Waste incinerators</t>
+  </si>
+  <si>
+    <t>(iii) Boilers of waste heat recovery system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(iv) Steam turbines, generators and
+condensers of waste heat
+recovery system </t>
+  </si>
+  <si>
+    <t>(v) Flue gas treatment facilities</t>
+  </si>
+  <si>
+    <t>(vi) Ash treatment facilities</t>
+  </si>
+  <si>
+    <t>(vii) Associated electrical works</t>
+  </si>
+  <si>
+    <t>(viii) Instrumentation and control works</t>
+  </si>
+  <si>
+    <t>(ix) Miscellaneous installations</t>
+  </si>
+  <si>
+    <t>(d) Mechanical and electrical works for other associated facilities</t>
+  </si>
+  <si>
+    <t>(e) Power connection, substation, associated facilities and installations of the power export system</t>
+  </si>
+  <si>
+    <t>(f) Transportation supporting facilities</t>
+  </si>
+  <si>
+    <t>(g) Mitigation measures and EM&amp;A for construction work</t>
+  </si>
+  <si>
+    <t>(h) Consultants’ fees for</t>
+  </si>
+  <si>
+    <t>(i)contract administration</t>
+  </si>
+  <si>
+    <t>(ii)management of resident site staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(i) Remuneration of resident site staff </t>
+  </si>
+  <si>
+    <t>(j) Contingencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-total 12,735.1 (in September
+2013 prices) </t>
+  </si>
+  <si>
+    <t>Sub-total in 2012 price</t>
+  </si>
+  <si>
+    <t>We adjust 2013 HKD to 2012 HKD using the following conversion factor:</t>
+  </si>
+  <si>
+    <t>2012 GDP</t>
+  </si>
+  <si>
+    <t>2013 GDP</t>
+  </si>
+  <si>
+    <t>At current market prices</t>
+  </si>
+  <si>
+    <t>In chained (2012) dollars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total  (in MOD
+prices) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(k) Provision for price adjustment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construction </t>
+  </si>
+  <si>
+    <t>2012 price</t>
+  </si>
+  <si>
+    <t>MSW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We estimate that the annual recurrent expenditure arising from the IWMF
+phase 1 to be about $402 million. The fees and charges implication arising from the
+project will be considered in the context of waste charging discussion. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">million </t>
+  </si>
+  <si>
+    <t>per year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the waste treatment process, the energy recovered will generate
+electricity for the use of IWMF phase 1. We plan to export the surplus electricity of
+about 480 million kWh2
+. </t>
+  </si>
+  <si>
+    <t>million KWH</t>
+  </si>
+  <si>
+    <t>We adjust 2013 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="###0;###0"/>
     <numFmt numFmtId="167" formatCode="###0.0;###0.0"/>
     <numFmt numFmtId="168" formatCode="###0.0"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1795,6 +1962,26 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1829,7 +2016,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2049,7 +2236,7 @@
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2222,13 +2409,27 @@
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2238,24 +2439,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: all except top row" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Header: top rows" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Footnotes: all except top row" xfId="9"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="2"/>
+    <cellStyle name="Header: top rows" xfId="10"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="3"/>
     <cellStyle name="Percent" xfId="14" builtinId="5"/>
-    <cellStyle name="Section Break" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Section Break: parent row" xfId="13" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Table title" xfId="1" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Section Break" xfId="12"/>
+    <cellStyle name="Section Break: parent row" xfId="13"/>
+    <cellStyle name="Table title" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2284,7 +2488,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Table Style 1" pivot="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2311,7 +2515,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>284952</xdr:colOff>
+      <xdr:colOff>218277</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>56500</xdr:rowOff>
     </xdr:to>
@@ -2338,6 +2542,50 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="6380952" cy="5200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>418465</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>18436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5790E47A-C3BA-4B50-BBE0-4B0FC040CC3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7639050" y="6343650"/>
+          <a:ext cx="5076190" cy="4914286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2425,23 +2673,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2477,23 +2708,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2669,23 +2883,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="91.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="56.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.7109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="2" max="2" width="91.3984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.3984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="56.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.73046875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2730,7 +2944,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="28.5">
       <c r="B8" s="53" t="s">
         <v>8</v>
       </c>
@@ -2782,7 +2996,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30">
+    <row r="15" spans="1:4" ht="28.5">
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2790,7 +3004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4">
       <c r="B16" s="66" t="s">
         <v>19</v>
       </c>
@@ -2855,7 +3069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="28.5">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
         <v>29</v>
@@ -3242,7 +3456,9 @@
       <c r="K60" s="8"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61"/>
+      <c r="A61" t="s">
+        <v>417</v>
+      </c>
       <c r="B61" s="7"/>
       <c r="D61" s="5"/>
       <c r="E61" s="8"/>
@@ -3254,8 +3470,8 @@
       <c r="K61" s="8"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" t="s">
-        <v>57</v>
+      <c r="A62">
+        <v>0.98599999999999999</v>
       </c>
       <c r="B62" s="7"/>
       <c r="D62" s="5"/>
@@ -3268,6 +3484,7 @@
       <c r="K62" s="8"/>
     </row>
     <row r="63" spans="1:11">
+      <c r="A63"/>
       <c r="B63" s="7"/>
       <c r="D63" s="5"/>
       <c r="E63" s="8"/>
@@ -3279,6 +3496,10 @@
       <c r="K63" s="8"/>
     </row>
     <row r="64" spans="1:11">
+      <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" s="7"/>
       <c r="D64" s="5"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
@@ -3300,7 +3521,6 @@
       <c r="K65" s="8"/>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="7"/>
       <c r="D66" s="5"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
@@ -3422,6 +3642,14 @@
     </row>
     <row r="77" spans="2:11">
       <c r="B77" s="7"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
     </row>
     <row r="78" spans="2:11">
       <c r="B78" s="7"/>
@@ -3436,14 +3664,6 @@
     </row>
     <row r="79" spans="2:11">
       <c r="B79" s="7"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
     </row>
     <row r="80" spans="2:11">
       <c r="B80" s="7"/>
@@ -3468,7 +3688,6 @@
       <c r="K81" s="8"/>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="5"/>
       <c r="B82" s="7"/>
       <c r="D82" s="5"/>
       <c r="E82" s="8"/>
@@ -3491,6 +3710,7 @@
       <c r="K83" s="8"/>
     </row>
     <row r="84" spans="1:11">
+      <c r="A84" s="5"/>
       <c r="B84" s="7"/>
       <c r="D84" s="5"/>
       <c r="E84" s="8"/>
@@ -3513,6 +3733,7 @@
       <c r="K85" s="8"/>
     </row>
     <row r="86" spans="1:11">
+      <c r="B86" s="7"/>
       <c r="D86" s="5"/>
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
@@ -3523,6 +3744,7 @@
       <c r="K86" s="8"/>
     </row>
     <row r="87" spans="1:11">
+      <c r="B87" s="7"/>
       <c r="D87" s="5"/>
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
@@ -3642,14 +3864,34 @@
       <c r="J98" s="8"/>
       <c r="K98" s="8"/>
     </row>
+    <row r="99" spans="4:11">
+      <c r="D99" s="5"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+    </row>
+    <row r="100" spans="4:11">
+      <c r="D100" s="5"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId3" display="http://www.irena.org/publications/2018/Jan/Renewable-power-generation-costs-in-2017" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A52" r:id="rId5" display="https://www.iea.org/statistics/?country=CHINA&amp;year=2016&amp;category=Electricity&amp;indicator=undefined&amp;mode=chart&amp;categoryBrowse=true&amp;dataTable=ELECTRICITYANDHEAT" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D16" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId3" display="http://www.irena.org/publications/2018/Jan/Renewable-power-generation-costs-in-2017"/>
+    <hyperlink ref="B30" r:id="rId4"/>
+    <hyperlink ref="A52" r:id="rId5" display="https://www.iea.org/statistics/?country=CHINA&amp;year=2016&amp;category=Electricity&amp;indicator=undefined&amp;mode=chart&amp;categoryBrowse=true&amp;dataTable=ELECTRICITYANDHEAT"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
@@ -3657,33 +3899,33 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" customWidth="1"/>
+    <col min="2" max="2" width="23.1328125" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>124</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>127</v>
@@ -3844,7 +4086,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11" s="4">
         <v>7340</v>
@@ -3875,7 +4117,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B13" s="4">
         <f>B2</f>
@@ -3909,7 +4151,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B15" s="4">
         <f>B11</f>
@@ -3925,7 +4167,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B16" s="4">
         <f>B11</f>
@@ -3941,18 +4183,18 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17" s="75">
-        <f>'MSW HK'!N9</f>
-        <v>14962453.333333334</v>
-      </c>
-      <c r="C17" s="73">
+        <v>351</v>
+      </c>
+      <c r="B17" s="4">
+        <f>'MSW HK'!N5*10^9/'MSW HK'!N7</f>
+        <v>473402.41959958256</v>
+      </c>
+      <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" s="72">
+      <c r="D17" s="4">
         <f>B17</f>
-        <v>14962453.333333334</v>
+        <v>473402.41959958256</v>
       </c>
     </row>
   </sheetData>
@@ -3963,31 +4205,31 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" customWidth="1"/>
     <col min="2" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>124</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>127</v>
@@ -4147,7 +4389,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11" s="69">
         <v>15.44</v>
@@ -4178,7 +4420,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B13" s="69">
         <f>B2</f>
@@ -4212,7 +4454,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B15" s="9">
         <f>B11</f>
@@ -4229,7 +4471,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B16" s="9">
         <f>B12</f>
@@ -4246,17 +4488,22 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17">
-        <v>8.49</v>
-      </c>
-      <c r="C17">
+        <v>351</v>
+      </c>
+      <c r="B17" s="85">
+        <f>'EIA Costs'!E16*About!$A$62</f>
+        <v>8.6176399999999997</v>
+      </c>
+      <c r="C17" s="86">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>8.49</v>
-      </c>
+      <c r="D17" s="85">
+        <f>B17</f>
+        <v>8.6176399999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="B18" s="82"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -4266,88 +4513,90 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="6" style="61" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="17.265625" style="61" customWidth="1"/>
     <col min="3" max="3" width="31" style="61" customWidth="1"/>
-    <col min="4" max="5" width="17.28515625" style="61" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="61" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="61" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="61" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="61" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" style="61" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" style="61" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" style="61" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="61" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="22.140625" style="61" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7109375" style="61"/>
+    <col min="4" max="5" width="17.265625" style="61" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" style="61" customWidth="1"/>
+    <col min="7" max="7" width="17.265625" style="61" customWidth="1"/>
+    <col min="8" max="8" width="22.59765625" style="61" customWidth="1"/>
+    <col min="9" max="9" width="17.265625" style="61" customWidth="1"/>
+    <col min="10" max="10" width="22.3984375" style="61" customWidth="1"/>
+    <col min="11" max="11" width="20.86328125" style="61" customWidth="1"/>
+    <col min="12" max="12" width="28.1328125" style="61" customWidth="1"/>
+    <col min="13" max="13" width="19.1328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="22.1328125" style="61" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1328125" style="74" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.73046875" style="61" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.73046875" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" ht="28.5">
       <c r="A1" s="60" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="60" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1" s="60" t="s">
         <v>354</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="D1" s="60" t="s">
         <v>355</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="E1" s="60" t="s">
         <v>356</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="F1" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="G1" s="60" t="s">
         <v>358</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="H1" s="60" t="s">
         <v>359</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="I1" s="60" t="s">
         <v>360</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="J1" s="60" t="s">
         <v>361</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="K1" s="60" t="s">
         <v>362</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="L1" s="60" t="s">
         <v>363</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="M1" s="60" t="s">
         <v>364</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="N1" s="60" t="s">
         <v>365</v>
       </c>
-      <c r="N1" s="60" t="s">
-        <v>366</v>
-      </c>
       <c r="O1" s="60" t="s">
+        <v>349</v>
+      </c>
+      <c r="P1" s="60" t="s">
         <v>350</v>
       </c>
-      <c r="P1" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q1" s="60" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="Q1" s="83" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="62">
         <v>2016</v>
       </c>
@@ -4410,11 +4659,13 @@
         <f>K2</f>
         <v>654224.44741861895</v>
       </c>
-      <c r="Q2" s="63">
-        <v>7982156.7055278737</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="Q2" s="84">
+        <f>'MSW HK'!N4*10^9/'MSW HK'!N7</f>
+        <v>9683361.5776772462</v>
+      </c>
+      <c r="R2" s="63"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="62">
         <v>2017</v>
       </c>
@@ -4477,11 +4728,12 @@
         <f t="shared" ref="P3:P36" si="1">K3</f>
         <v>654225.44741861895</v>
       </c>
-      <c r="Q3" s="63">
-        <v>7971502.811055745</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="Q3" s="84">
+        <f>Q2</f>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="62">
         <v>2018</v>
       </c>
@@ -4544,11 +4796,12 @@
         <f t="shared" si="1"/>
         <v>652272.3387205411</v>
       </c>
-      <c r="Q4" s="63">
-        <v>7982156.7055278737</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="Q4" s="84">
+        <f t="shared" ref="Q4:Q10" si="3">Q3</f>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="62">
         <v>2019</v>
       </c>
@@ -4611,11 +4864,12 @@
         <f t="shared" si="1"/>
         <v>649811.88595093053</v>
       </c>
-      <c r="Q5" s="63">
-        <v>7971502.811055745</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="Q5" s="84">
+        <f t="shared" si="3"/>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="62">
         <v>2020</v>
       </c>
@@ -4678,11 +4932,12 @@
         <f t="shared" si="1"/>
         <v>645390.95246922853</v>
       </c>
-      <c r="Q6" s="63">
-        <v>7958626.596631432</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="Q6" s="84">
+        <f t="shared" si="3"/>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="62">
         <v>2021</v>
       </c>
@@ -4745,11 +5000,12 @@
         <f t="shared" si="1"/>
         <v>643437.69417805946</v>
       </c>
-      <c r="Q7" s="63">
-        <v>8047515.0385973537</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="Q7" s="84">
+        <f t="shared" si="3"/>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="62">
         <v>2022</v>
       </c>
@@ -4812,11 +5068,12 @@
         <f t="shared" si="1"/>
         <v>641442.67327765853</v>
       </c>
-      <c r="Q8" s="63">
-        <v>7840906.0539358519</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8" s="84">
+        <f t="shared" si="3"/>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="62">
         <v>2023</v>
       </c>
@@ -4879,11 +5136,12 @@
         <f t="shared" si="1"/>
         <v>639489.166581125</v>
       </c>
-      <c r="Q9" s="63">
-        <v>7803020.8428130085</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9" s="84">
+        <f t="shared" si="3"/>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="62">
         <v>2024</v>
       </c>
@@ -4946,11 +5204,12 @@
         <f t="shared" si="1"/>
         <v>637536.40933158563</v>
       </c>
-      <c r="Q10" s="63">
-        <v>7768616.5588959409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="Q10" s="84">
+        <f t="shared" si="3"/>
+        <v>9683361.5776772462</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="62">
         <v>2025</v>
       </c>
@@ -5013,11 +5272,12 @@
         <f t="shared" si="1"/>
         <v>635482.86120436469</v>
       </c>
-      <c r="Q11" s="63">
-        <v>7764569.8125896389</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="Q11" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A11,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9383430.4925892297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="62">
         <v>2026</v>
       </c>
@@ -5080,11 +5340,12 @@
         <f t="shared" si="1"/>
         <v>629014.61231266905</v>
       </c>
-      <c r="Q12" s="63">
-        <v>7757634.4939132584</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q12" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A12,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9356645.6240954902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="62">
         <v>2027</v>
       </c>
@@ -5147,11 +5408,12 @@
         <f t="shared" si="1"/>
         <v>624104.63841106219</v>
       </c>
-      <c r="Q13" s="63">
-        <v>7746868.1516131693</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="Q13" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A13,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9329853.8267850615</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="62">
         <v>2028</v>
       </c>
@@ -5214,11 +5476,12 @@
         <f t="shared" si="1"/>
         <v>619575.81905558321</v>
       </c>
-      <c r="Q14" s="63">
-        <v>7728499.6649701986</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="Q14" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A14,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9303061.3560645226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="62">
         <v>2029</v>
       </c>
@@ -5281,11 +5544,12 @@
         <f t="shared" si="1"/>
         <v>616448.38075626816</v>
       </c>
-      <c r="Q15" s="63">
-        <v>7694951.9782399936</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="Q15" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A15,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9276277.187211372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="62">
         <v>2030</v>
       </c>
@@ -5348,8 +5612,9 @@
         <f t="shared" si="1"/>
         <v>613103.989995774</v>
       </c>
-      <c r="Q16" s="63">
-        <v>7673261.2195788976</v>
+      <c r="Q16" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A16,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9249484.9326015376</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -5415,8 +5680,9 @@
         <f t="shared" si="1"/>
         <v>610100.70335621736</v>
       </c>
-      <c r="Q17" s="63">
-        <v>7651766.5026455559</v>
+      <c r="Q17" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A17,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9222687.933625862</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -5482,8 +5748,9 @@
         <f t="shared" si="1"/>
         <v>607777.3086571634</v>
       </c>
-      <c r="Q18" s="63">
-        <v>7626303.7360194027</v>
+      <c r="Q18" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A18,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9195901.6852810681</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -5549,8 +5816,9 @@
         <f t="shared" si="1"/>
         <v>605748.1000457817</v>
       </c>
-      <c r="Q19" s="63">
-        <v>7603867.4320185054</v>
+      <c r="Q19" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A19,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9169114.6061549317</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -5616,8 +5884,9 @@
         <f t="shared" si="1"/>
         <v>603684.81012468517</v>
       </c>
-      <c r="Q20" s="63">
-        <v>7587101.1716198716</v>
+      <c r="Q20" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A20,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9142323.459139768</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -5683,8 +5952,9 @@
         <f t="shared" si="1"/>
         <v>601330.37504906254</v>
       </c>
-      <c r="Q21" s="63">
-        <v>7561294.8637536224</v>
+      <c r="Q21" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A21,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9115531.9516623393</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -5750,8 +6020,9 @@
         <f t="shared" si="1"/>
         <v>598957.8048655868</v>
       </c>
-      <c r="Q22" s="63">
-        <v>7538547.4766855622</v>
+      <c r="Q22" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A22,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9088738.3691054042</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -5817,8 +6088,9 @@
         <f t="shared" si="1"/>
         <v>596955.4197425656</v>
       </c>
-      <c r="Q23" s="63">
-        <v>7514086.0827102391</v>
+      <c r="Q23" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A23,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9061950.6935845464</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -5884,8 +6156,9 @@
         <f t="shared" si="1"/>
         <v>594440.08024455211</v>
       </c>
-      <c r="Q24" s="63">
-        <v>7493538.9828844583</v>
+      <c r="Q24" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A24,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9035158.8301438484</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -5951,8 +6224,9 @@
         <f t="shared" si="1"/>
         <v>592434.16432381817</v>
       </c>
-      <c r="Q25" s="63">
-        <v>7469211.21148971</v>
+      <c r="Q25" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A25,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>9008371.9235372487</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -6018,8 +6292,9 @@
         <f t="shared" si="1"/>
         <v>590089.47107294935</v>
       </c>
-      <c r="Q26" s="63">
-        <v>7445775.4433545973</v>
+      <c r="Q26" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A26,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8981575.6644978654</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -6085,8 +6360,9 @@
         <f t="shared" si="1"/>
         <v>587788.019180667</v>
       </c>
-      <c r="Q27" s="63">
-        <v>7429595.5857021902</v>
+      <c r="Q27" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A27,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8954784.7376875002</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -6152,8 +6428,9 @@
         <f t="shared" si="1"/>
         <v>585486.56728838454</v>
       </c>
-      <c r="Q28" s="63">
-        <v>7397570.8487657513</v>
+      <c r="Q28" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A28,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8927993.8108771313</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -6219,8 +6496,9 @@
         <f t="shared" si="1"/>
         <v>583185.11539610196</v>
       </c>
-      <c r="Q29" s="63">
-        <v>7385036.9682956832</v>
+      <c r="Q29" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A29,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8901202.8840667661</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -6286,8 +6564,9 @@
         <f t="shared" si="1"/>
         <v>580883.66350381961</v>
       </c>
-      <c r="Q30" s="63">
-        <v>7354522.1212749518</v>
+      <c r="Q30" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A30,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8874411.9572563972</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -6353,8 +6632,9 @@
         <f t="shared" si="1"/>
         <v>578582.21161153703</v>
       </c>
-      <c r="Q31" s="63">
-        <v>7340437.2226737272</v>
+      <c r="Q31" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A31,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8847621.0304460321</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -6420,8 +6700,9 @@
         <f t="shared" si="1"/>
         <v>576280.75971925457</v>
       </c>
-      <c r="Q32" s="63">
-        <v>7312648.7933935076</v>
+      <c r="Q32" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A32,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8820830.1036356632</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -6487,8 +6768,9 @@
         <f t="shared" si="1"/>
         <v>573979.3078269721</v>
       </c>
-      <c r="Q33" s="63">
-        <v>7291302.5022382103</v>
+      <c r="Q33" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A33,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8794039.176825298</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -6554,8 +6836,9 @@
         <f t="shared" si="1"/>
         <v>571677.85593468964</v>
       </c>
-      <c r="Q34" s="63">
-        <v>7269844.3251363151</v>
+      <c r="Q34" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A34,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8767248.2500149291</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -6621,8 +6904,9 @@
         <f t="shared" si="1"/>
         <v>569376.40404240706</v>
       </c>
-      <c r="Q35" s="63">
-        <v>7247772.4406001931</v>
+      <c r="Q35" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A35,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8740457.3232045621</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -6688,8 +6972,9 @@
         <f t="shared" si="1"/>
         <v>567074.95215012471</v>
       </c>
-      <c r="Q36" s="63">
-        <v>7173106.1111970115</v>
+      <c r="Q36" s="84">
+        <f>$Q$10*INDEX('Cost Improvement (other)'!$B$118:$AL$124,MATCH("biomass",'Cost Improvement (other)'!$A$118:$A$124,0),MATCH('CCaMC-BCCpUC'!$A36,'Cost Improvement (other)'!$B$117:$AL$117,0))</f>
+        <v>8713666.396394195</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -6734,45 +7019,46 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" customWidth="1"/>
+    <col min="5" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="7.86328125" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77" t="s">
+      <c r="E1" s="87"/>
+      <c r="F1" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="77"/>
+      <c r="G1" s="87"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="77"/>
+      <c r="A2" s="87"/>
       <c r="B2" t="s">
         <v>62</v>
       </c>
@@ -6966,19 +7252,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.86328125" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" customWidth="1"/>
+    <col min="3" max="3" width="20.1328125" customWidth="1"/>
+    <col min="4" max="4" width="16.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -7050,7 +7336,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="1:11" ht="28.5">
+    <row r="7" spans="1:11" ht="27">
       <c r="A7" s="13"/>
       <c r="B7" s="14" t="s">
         <v>81</v>
@@ -7063,7 +7349,7 @@
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:11" ht="57">
+    <row r="8" spans="1:11" ht="40.5">
       <c r="A8" s="14" t="s">
         <v>83</v>
       </c>
@@ -7378,7 +7664,7 @@
       <c r="K23" s="55"/>
       <c r="L23" s="55"/>
     </row>
-    <row r="24" spans="1:12" ht="42.75">
+    <row r="24" spans="1:12" ht="40.5">
       <c r="A24" s="56" t="s">
         <v>102</v>
       </c>
@@ -7950,19 +8236,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.3984375" customWidth="1"/>
+    <col min="2" max="2" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="20.1328125" customWidth="1"/>
+    <col min="4" max="4" width="19.265625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8014,21 +8300,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="34.73046875" customWidth="1"/>
+    <col min="4" max="4" width="34.3984375" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8432,24 +8718,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.86328125" customWidth="1"/>
+    <col min="11" max="11" width="8.86328125" customWidth="1"/>
+    <col min="12" max="12" width="15.59765625" customWidth="1"/>
+    <col min="13" max="13" width="11.59765625" customWidth="1"/>
+    <col min="14" max="14" width="12.73046875" customWidth="1"/>
+    <col min="15" max="15" width="12.59765625" customWidth="1"/>
+    <col min="16" max="16" width="13.59765625" customWidth="1"/>
+    <col min="17" max="17" width="10.86328125" customWidth="1"/>
+    <col min="18" max="18" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="55.5" customHeight="1">
@@ -8612,7 +8898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="24">
+    <row r="5" spans="1:18" ht="23.25">
       <c r="A5" s="22"/>
       <c r="B5" s="24" t="s">
         <v>170</v>
@@ -8637,6 +8923,9 @@
       </c>
       <c r="I5" s="24" t="s">
         <v>176</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -8840,17 +9129,17 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="88" t="s">
         <v>194</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="36" t="s">
@@ -9136,17 +9425,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM124"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView topLeftCell="T109" workbookViewId="0">
+      <selection activeCell="AL124" sqref="AL124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
@@ -23793,35 +24082,35 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="17"/>
-    <col min="3" max="3" width="18.5703125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="8.73046875" style="17"/>
+    <col min="3" max="3" width="18.59765625" style="17" customWidth="1"/>
     <col min="4" max="4" width="15" style="17" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" customWidth="1"/>
+    <col min="10" max="10" width="14.59765625" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="89" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="89" t="s">
         <v>322</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="89" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="79"/>
+      <c r="D1" s="89"/>
       <c r="I1" t="s">
         <v>324</v>
       </c>
@@ -23835,13 +24124,13 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
-      <c r="A2" s="79"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="76" t="s">
+    <row r="2" spans="1:12" ht="28.5">
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="72" t="s">
         <v>328</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="72" t="s">
         <v>329</v>
       </c>
       <c r="H2">
@@ -23861,16 +24150,16 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="89" t="s">
         <v>330</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="72">
         <v>2010</v>
       </c>
-      <c r="C3" s="79">
+      <c r="C3" s="89">
         <v>1.2</v>
       </c>
-      <c r="D3" s="79"/>
+      <c r="D3" s="89"/>
       <c r="H3">
         <v>2011</v>
       </c>
@@ -23892,14 +24181,14 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="79"/>
-      <c r="B4" s="76">
+      <c r="A4" s="89"/>
+      <c r="B4" s="72">
         <v>2020</v>
       </c>
-      <c r="C4" s="76">
+      <c r="C4" s="72">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="72">
         <v>0.6</v>
       </c>
       <c r="H4">
@@ -23923,14 +24212,14 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="79"/>
-      <c r="B5" s="76">
+      <c r="A5" s="89"/>
+      <c r="B5" s="72">
         <v>2030</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="72">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="72">
         <v>0.6</v>
       </c>
       <c r="H5">
@@ -23954,14 +24243,14 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="79"/>
-      <c r="B6" s="76">
+      <c r="A6" s="89"/>
+      <c r="B6" s="72">
         <v>2050</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="72">
         <v>1</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="72">
         <v>0.6</v>
       </c>
       <c r="H6">
@@ -23985,16 +24274,16 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="89" t="s">
         <v>331</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="72">
         <v>2010</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="89">
         <v>3</v>
       </c>
-      <c r="D7" s="79"/>
+      <c r="D7" s="89"/>
       <c r="H7">
         <v>2015</v>
       </c>
@@ -24016,14 +24305,14 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="79"/>
-      <c r="B8" s="76">
+      <c r="A8" s="89"/>
+      <c r="B8" s="72">
         <v>2020</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="72">
         <v>2.25</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="72">
         <v>1.5</v>
       </c>
       <c r="H8">
@@ -24047,14 +24336,14 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="79"/>
-      <c r="B9" s="76">
+      <c r="A9" s="89"/>
+      <c r="B9" s="72">
         <v>2030</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="72">
         <v>2.15</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="72">
         <v>1.5</v>
       </c>
       <c r="H9">
@@ -24078,14 +24367,14 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="79"/>
-      <c r="B10" s="76">
+      <c r="A10" s="89"/>
+      <c r="B10" s="72">
         <v>2050</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="72">
         <v>2</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="72">
         <v>1.5</v>
       </c>
       <c r="H10">
@@ -24109,16 +24398,16 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="89" t="s">
         <v>332</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="72">
         <v>2010</v>
       </c>
-      <c r="C11" s="79">
+      <c r="C11" s="89">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D11" s="79"/>
+      <c r="D11" s="89"/>
       <c r="H11">
         <v>2019</v>
       </c>
@@ -24140,14 +24429,14 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="79"/>
-      <c r="B12" s="76">
+      <c r="A12" s="89"/>
+      <c r="B12" s="72">
         <v>2020</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="72">
         <v>1.2</v>
       </c>
-      <c r="D12" s="76">
+      <c r="D12" s="72">
         <v>1</v>
       </c>
       <c r="H12">
@@ -24171,14 +24460,14 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="79"/>
-      <c r="B13" s="76">
+      <c r="A13" s="89"/>
+      <c r="B13" s="72">
         <v>2030</v>
       </c>
-      <c r="C13" s="76">
+      <c r="C13" s="72">
         <v>1.2</v>
       </c>
-      <c r="D13" s="76">
+      <c r="D13" s="72">
         <v>1</v>
       </c>
       <c r="H13">
@@ -24202,14 +24491,14 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="79"/>
-      <c r="B14" s="76">
+      <c r="A14" s="89"/>
+      <c r="B14" s="72">
         <v>2050</v>
       </c>
-      <c r="C14" s="76">
+      <c r="C14" s="72">
         <v>1.2</v>
       </c>
-      <c r="D14" s="76">
+      <c r="D14" s="72">
         <v>1</v>
       </c>
       <c r="H14">
@@ -24233,16 +24522,16 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="89" t="s">
         <v>333</v>
       </c>
-      <c r="B15" s="76">
+      <c r="B15" s="72">
         <v>2010</v>
       </c>
-      <c r="C15" s="79">
+      <c r="C15" s="89">
         <v>2.5</v>
       </c>
-      <c r="D15" s="79"/>
+      <c r="D15" s="89"/>
       <c r="H15">
         <v>2023</v>
       </c>
@@ -24264,14 +24553,14 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="79"/>
-      <c r="B16" s="76">
+      <c r="A16" s="89"/>
+      <c r="B16" s="72">
         <v>2020</v>
       </c>
-      <c r="C16" s="76">
+      <c r="C16" s="72">
         <v>1.5</v>
       </c>
-      <c r="D16" s="76">
+      <c r="D16" s="72">
         <v>1.25</v>
       </c>
       <c r="H16">
@@ -24295,14 +24584,14 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="79"/>
-      <c r="B17" s="76">
+      <c r="A17" s="89"/>
+      <c r="B17" s="72">
         <v>2030</v>
       </c>
-      <c r="C17" s="76">
+      <c r="C17" s="72">
         <v>1.5</v>
       </c>
-      <c r="D17" s="76">
+      <c r="D17" s="72">
         <v>1.25</v>
       </c>
       <c r="H17">
@@ -24326,14 +24615,14 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="79"/>
-      <c r="B18" s="76">
+      <c r="A18" s="89"/>
+      <c r="B18" s="72">
         <v>2050</v>
       </c>
-      <c r="C18" s="76">
+      <c r="C18" s="72">
         <v>1.5</v>
       </c>
-      <c r="D18" s="76">
+      <c r="D18" s="72">
         <v>1.25</v>
       </c>
       <c r="H18">
@@ -24357,16 +24646,16 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="89" t="s">
         <v>334</v>
       </c>
-      <c r="B19" s="76">
+      <c r="B19" s="72">
         <v>2010</v>
       </c>
-      <c r="C19" s="79">
+      <c r="C19" s="89">
         <v>2.9</v>
       </c>
-      <c r="D19" s="79"/>
+      <c r="D19" s="89"/>
       <c r="H19">
         <v>2027</v>
       </c>
@@ -24388,14 +24677,14 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="79"/>
-      <c r="B20" s="76">
+      <c r="A20" s="89"/>
+      <c r="B20" s="72">
         <v>2020</v>
       </c>
-      <c r="C20" s="76">
+      <c r="C20" s="72">
         <v>2.5</v>
       </c>
-      <c r="D20" s="76">
+      <c r="D20" s="72">
         <v>1.5</v>
       </c>
       <c r="H20">
@@ -24419,14 +24708,14 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="79"/>
-      <c r="B21" s="76">
+      <c r="A21" s="89"/>
+      <c r="B21" s="72">
         <v>2030</v>
       </c>
-      <c r="C21" s="76">
+      <c r="C21" s="72">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D21" s="76">
+      <c r="D21" s="72">
         <v>1.5</v>
       </c>
       <c r="H21">
@@ -24450,14 +24739,14 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="79"/>
-      <c r="B22" s="76">
+      <c r="A22" s="89"/>
+      <c r="B22" s="72">
         <v>2050</v>
       </c>
-      <c r="C22" s="76">
+      <c r="C22" s="72">
         <v>2.1</v>
       </c>
-      <c r="D22" s="76">
+      <c r="D22" s="72">
         <v>1.5</v>
       </c>
       <c r="H22">
@@ -24481,16 +24770,16 @@
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="89" t="s">
         <v>335</v>
       </c>
-      <c r="B23" s="76">
+      <c r="B23" s="72">
         <v>2010</v>
       </c>
-      <c r="C23" s="79">
+      <c r="C23" s="89">
         <v>5</v>
       </c>
-      <c r="D23" s="79"/>
+      <c r="D23" s="89"/>
       <c r="H23">
         <v>2031</v>
       </c>
@@ -24512,14 +24801,14 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="79"/>
-      <c r="B24" s="76">
+      <c r="A24" s="89"/>
+      <c r="B24" s="72">
         <v>2020</v>
       </c>
-      <c r="C24" s="76">
+      <c r="C24" s="72">
         <v>4.5</v>
       </c>
-      <c r="D24" s="76">
+      <c r="D24" s="72">
         <v>2.5</v>
       </c>
       <c r="H24">
@@ -24543,14 +24832,14 @@
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="79"/>
-      <c r="B25" s="76">
+      <c r="A25" s="89"/>
+      <c r="B25" s="72">
         <v>2030</v>
       </c>
-      <c r="C25" s="76">
+      <c r="C25" s="72">
         <v>4</v>
       </c>
-      <c r="D25" s="76">
+      <c r="D25" s="72">
         <v>2.5</v>
       </c>
       <c r="H25">
@@ -24574,14 +24863,14 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="79"/>
-      <c r="B26" s="76">
+      <c r="A26" s="89"/>
+      <c r="B26" s="72">
         <v>2050</v>
       </c>
-      <c r="C26" s="76">
+      <c r="C26" s="72">
         <v>3.5</v>
       </c>
-      <c r="D26" s="76">
+      <c r="D26" s="72">
         <v>2.5</v>
       </c>
       <c r="H26">
@@ -24605,16 +24894,16 @@
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="89" t="s">
         <v>336</v>
       </c>
-      <c r="B27" s="76">
+      <c r="B27" s="72">
         <v>2010</v>
       </c>
-      <c r="C27" s="79">
+      <c r="C27" s="89">
         <v>6.5</v>
       </c>
-      <c r="D27" s="79"/>
+      <c r="D27" s="89"/>
       <c r="H27">
         <v>2035</v>
       </c>
@@ -24636,14 +24925,14 @@
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="79"/>
-      <c r="B28" s="76">
+      <c r="A28" s="89"/>
+      <c r="B28" s="72">
         <v>2020</v>
       </c>
-      <c r="C28" s="76">
+      <c r="C28" s="72">
         <v>4.8</v>
       </c>
-      <c r="D28" s="76">
+      <c r="D28" s="72">
         <v>3.07</v>
       </c>
       <c r="H28">
@@ -24667,14 +24956,14 @@
       </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="79"/>
-      <c r="B29" s="76">
+      <c r="A29" s="89"/>
+      <c r="B29" s="72">
         <v>2030</v>
       </c>
-      <c r="C29" s="76">
+      <c r="C29" s="72">
         <v>4</v>
       </c>
-      <c r="D29" s="76">
+      <c r="D29" s="72">
         <v>3.07</v>
       </c>
       <c r="H29">
@@ -24698,14 +24987,14 @@
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="79"/>
-      <c r="B30" s="76">
+      <c r="A30" s="89"/>
+      <c r="B30" s="72">
         <v>2050</v>
       </c>
-      <c r="C30" s="76">
+      <c r="C30" s="72">
         <v>3.6</v>
       </c>
-      <c r="D30" s="76">
+      <c r="D30" s="72">
         <v>3.07</v>
       </c>
       <c r="H30">
@@ -24729,10 +25018,10 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="76"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
       <c r="H31">
         <v>2039</v>
       </c>
@@ -24754,10 +25043,10 @@
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
       <c r="H32">
         <v>2040</v>
       </c>
@@ -24990,6 +25279,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C3:D3"/>
@@ -25002,11 +25296,6 @@
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25014,74 +25303,83 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337F4D1D-3FBA-4E74-8B3D-8AD70E04A037}">
-  <dimension ref="M1:S9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T77"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="13" max="13" width="12.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.59765625" customWidth="1"/>
+    <col min="14" max="14" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.3984375" customWidth="1"/>
+    <col min="20" max="20" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="13:19">
+    <row r="1" spans="13:20">
       <c r="M1" t="s">
         <v>337</v>
       </c>
-      <c r="N1">
-        <v>18.010000000000002</v>
+      <c r="N1" s="11">
+        <f>I66/1000</f>
+        <v>12.521588246996441</v>
       </c>
       <c r="O1" t="s">
         <v>338</v>
       </c>
       <c r="Q1" t="s">
+        <v>410</v>
+      </c>
+      <c r="R1" t="s">
         <v>339</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>0.12759999999999999</v>
       </c>
     </row>
-    <row r="2" spans="13:19">
+    <row r="2" spans="13:20">
       <c r="M2" t="s">
         <v>340</v>
       </c>
-      <c r="N2">
-        <f>13.38/10</f>
-        <v>1.3380000000000001</v>
+      <c r="N2" s="11">
+        <f>13.38/15*(N1*1000/I65)</f>
+        <v>0.61215830120635684</v>
       </c>
       <c r="O2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="4" spans="13:19">
+      <c r="Q2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" spans="13:20">
       <c r="M4" t="s">
         <v>337</v>
       </c>
-      <c r="N4">
-        <f>N1*S1</f>
-        <v>2.298076</v>
+      <c r="N4" s="11">
+        <f>N1*T1</f>
+        <v>1.5977546603167456</v>
       </c>
       <c r="O4" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="13:19">
+    <row r="5" spans="13:20">
       <c r="M5" t="s">
         <v>340</v>
       </c>
-      <c r="N5">
-        <f>N2*S1</f>
-        <v>0.17072879999999999</v>
+      <c r="N5" s="11">
+        <f>N2*T1</f>
+        <v>7.8111399233931122E-2</v>
       </c>
       <c r="O5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="13:19">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="13:20">
       <c r="M7" t="s">
         <v>343</v>
       </c>
@@ -25092,47 +25390,542 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="13:19">
-      <c r="M9" t="s">
-        <v>345</v>
-      </c>
-      <c r="N9" s="74">
-        <f>SUM(N4:N5)*10^9/N7</f>
-        <v>14962453.333333334</v>
+    <row r="9" spans="13:20">
+      <c r="N9" s="73"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="75" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="75" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="I34" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="77" t="s">
+        <v>372</v>
+      </c>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="79">
+        <v>2434.4</v>
+      </c>
+      <c r="K35" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="76" t="s">
+        <v>373</v>
+      </c>
+      <c r="I36" s="78">
+        <v>1081.5999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="76" t="s">
+        <v>374</v>
+      </c>
+      <c r="I37" s="78">
+        <v>904.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="76" t="s">
+        <v>375</v>
+      </c>
+      <c r="I38" s="78">
+        <v>448.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="77" t="s">
+        <v>376</v>
+      </c>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="79">
+        <v>1139.0999999999999</v>
+      </c>
+      <c r="K39" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="76" t="s">
+        <v>377</v>
+      </c>
+      <c r="I40" s="78">
+        <v>843.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="76" t="s">
+        <v>378</v>
+      </c>
+      <c r="I41" s="78">
+        <v>125.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="76" t="s">
+        <v>379</v>
+      </c>
+      <c r="I42" s="78">
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="76" t="s">
+        <v>380</v>
+      </c>
+      <c r="I43" s="78">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="77" t="s">
+        <v>381</v>
+      </c>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="79">
+        <v>6407.2</v>
+      </c>
+      <c r="K44" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="76" t="s">
+        <v>382</v>
+      </c>
+      <c r="I45" s="78">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="76" t="s">
+        <v>383</v>
+      </c>
+      <c r="I46" s="78">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="76" t="s">
+        <v>384</v>
+      </c>
+      <c r="I47" s="78">
+        <v>1171.0999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="76" t="s">
+        <v>385</v>
+      </c>
+      <c r="I48" s="78">
+        <v>850.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="76" t="s">
+        <v>386</v>
+      </c>
+      <c r="I49" s="78">
+        <v>948.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="76" t="s">
+        <v>387</v>
+      </c>
+      <c r="I50" s="78">
+        <v>439.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="76" t="s">
+        <v>388</v>
+      </c>
+      <c r="I51" s="78">
+        <v>854.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="76" t="s">
+        <v>389</v>
+      </c>
+      <c r="I52" s="78">
+        <v>319.89999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="76" t="s">
+        <v>390</v>
+      </c>
+      <c r="I53" s="78">
+        <v>520.79999999999995</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="77" t="s">
+        <v>391</v>
+      </c>
+      <c r="B54" s="77"/>
+      <c r="C54" s="77"/>
+      <c r="D54" s="77"/>
+      <c r="E54" s="77"/>
+      <c r="F54" s="77"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="77"/>
+      <c r="I54" s="79">
+        <v>311.39999999999998</v>
+      </c>
+      <c r="K54" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="77" t="s">
+        <v>392</v>
+      </c>
+      <c r="B55" s="77"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="77"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="79">
+        <v>774.3</v>
+      </c>
+      <c r="K55" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="77" t="s">
+        <v>393</v>
+      </c>
+      <c r="B56" s="77"/>
+      <c r="C56" s="77"/>
+      <c r="D56" s="77"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="77"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="77"/>
+      <c r="I56" s="79">
+        <v>277.3</v>
+      </c>
+      <c r="K56" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="77" t="s">
+        <v>394</v>
+      </c>
+      <c r="B57" s="77"/>
+      <c r="C57" s="77"/>
+      <c r="D57" s="77"/>
+      <c r="E57" s="77"/>
+      <c r="F57" s="77"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="77"/>
+      <c r="I57" s="79">
+        <v>127</v>
+      </c>
+      <c r="K57" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="77" t="s">
+        <v>395</v>
+      </c>
+      <c r="B58" s="77"/>
+      <c r="C58" s="77"/>
+      <c r="D58" s="77"/>
+      <c r="E58" s="77"/>
+      <c r="F58" s="77"/>
+      <c r="G58" s="77"/>
+      <c r="H58" s="77"/>
+      <c r="I58" s="79">
+        <v>52.9</v>
+      </c>
+      <c r="K58" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="76" t="s">
+        <v>396</v>
+      </c>
+      <c r="I59" s="78">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="76" t="s">
+        <v>397</v>
+      </c>
+      <c r="I60" s="78">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="77" t="s">
+        <v>398</v>
+      </c>
+      <c r="B61" s="77"/>
+      <c r="C61" s="77"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="77"/>
+      <c r="F61" s="77"/>
+      <c r="G61" s="77"/>
+      <c r="H61" s="77"/>
+      <c r="I61" s="79">
+        <v>159.1</v>
+      </c>
+      <c r="K61" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="B62" s="77"/>
+      <c r="C62" s="77"/>
+      <c r="D62" s="77"/>
+      <c r="E62" s="77"/>
+      <c r="F62" s="77"/>
+      <c r="G62" s="77"/>
+      <c r="H62" s="77"/>
+      <c r="I62" s="79">
+        <v>1052.4000000000001</v>
+      </c>
+      <c r="K62" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="75" t="s">
+        <v>400</v>
+      </c>
+      <c r="I63" s="78">
+        <f>I35+I39+I44+SUM(I54:I58)+I61+I62</f>
+        <v>12735.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" t="s">
+        <v>408</v>
+      </c>
+      <c r="I64" s="78">
+        <v>5510.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="75" t="s">
+        <v>407</v>
+      </c>
+      <c r="I65" s="78">
+        <v>18245.7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="80" t="s">
+        <v>401</v>
+      </c>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18">
+        <f>I63*A69</f>
+        <v>12521.58824699644</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="80"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69">
+        <f>G72/B72</f>
+        <v>0.9832343874014684</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>405</v>
+      </c>
+      <c r="F70" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>403</v>
+      </c>
+      <c r="B71" t="s">
+        <v>404</v>
+      </c>
+      <c r="F71" t="s">
+        <v>403</v>
+      </c>
+      <c r="G71" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="81">
+        <v>2037059</v>
+      </c>
+      <c r="B72" s="81">
+        <v>2131804</v>
+      </c>
+      <c r="F72" s="81">
+        <v>2037059</v>
+      </c>
+      <c r="G72" s="81">
+        <v>2096063</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="50.25" customHeight="1">
+      <c r="A74" s="90" t="s">
+        <v>412</v>
+      </c>
+      <c r="B74" s="90"/>
+      <c r="C74" s="90"/>
+      <c r="D74" s="90"/>
+      <c r="E74" s="90"/>
+      <c r="F74" s="90"/>
+      <c r="G74" s="90"/>
+      <c r="H74" s="90"/>
+      <c r="I74" s="90"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75">
+        <v>402</v>
+      </c>
+      <c r="B75" t="s">
+        <v>413</v>
+      </c>
+      <c r="C75" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="63.75" customHeight="1">
+      <c r="A76" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="B76" s="90"/>
+      <c r="C76" s="90"/>
+      <c r="D76" s="90"/>
+      <c r="E76" s="90"/>
+      <c r="F76" s="90"/>
+      <c r="G76" s="90"/>
+      <c r="H76" s="90"/>
+      <c r="I76" s="90"/>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77">
+        <v>480</v>
+      </c>
+      <c r="B77" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A74:I74"/>
+    <mergeCell ref="A76:I76"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A30" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
-    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
-    <xsd:import namespace="7889d872-e2a2-4afb-87bc-97561eced75f"/>
-    <xsd:import namespace="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005D5DE895D8AE54A972C2171818FD093" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85f6924c4aafd897c3f23384ae9dc35">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01f24951-2a3e-4fd5-a813-71a74687f653" xmlns:ns3="80a27e12-bb1f-4e28-b766-51f62aa5c67e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11afb4ea5aef950dd888cd3ab39ccec1" ns2:_="" ns3:_="">
+    <xsd:import namespace="01f24951-2a3e-4fd5-a813-71a74687f653"/>
+    <xsd:import namespace="80a27e12-bb1f-4e28-b766-51f62aa5c67e"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -25140,24 +25933,68 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="01f24951-2a3e-4fd5-a813-71a74687f653" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="18" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="19" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7889d872-e2a2-4afb-87bc-97561eced75f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="80a27e12-bb1f-4e28-b766-51f62aa5c67e" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -25176,65 +26013,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c9df191c-55f2-496b-9838-9a5abe4742ad" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="14" nillable="true" ma:displayName="MediaServiceLocation" ma:description="" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="20" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="21" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -25341,32 +26120,52 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
+  <documentManagement/>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F753106C-6C96-40DB-989F-DDACB7271E62}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53D4B8D-07E4-480A-9102-59E43F1C6BD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53D4B8D-07E4-480A-9102-59E43F1C6BD5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7130935E-3288-4243-8272-3335D81BE387}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="01f24951-2a3e-4fd5-a813-71a74687f653"/>
+    <ds:schemaRef ds:uri="80a27e12-bb1f-4e28-b766-51f62aa5c67e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666A01E7-B2FB-4480-B432-5D73735A58CA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666A01E7-B2FB-4480-B432-5D73735A58CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="80a27e12-bb1f-4e28-b766-51f62aa5c67e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="01f24951-2a3e-4fd5-a813-71a74687f653"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>